<commit_message>
Added my section to activity log
</commit_message>
<xml_diff>
--- a/Agora Team Activity Log.xlsx
+++ b/Agora Team Activity Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cedricstephani/Documents/INFO301/agora_student_marketplace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df8c00b68312d67f/University 2020 S2/INFO301/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFDD946-786A-BE40-A659-F92B6E369D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{486100A1-C139-4CF8-9454-35E6B6BB17A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="14280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
     <t>Idea selection, planning and overview of functionality, target audience and use case.</t>
   </si>
   <si>
-    <t>Collaborated on user studies</t>
+    <t>Gave instructions on how to download Microsoft Visual Code, ReactJS, Node.JS and MongoDB. Create starting React project base structure and push to Git. Ensure all group members can pull the project and run the react App in their browser. Assist with scheduling and delegating of stories.</t>
   </si>
 </sst>
 </file>
@@ -423,18 +423,18 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.6640625" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="6" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="24.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
@@ -452,7 +452,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -472,7 +472,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -492,19 +492,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -514,7 +514,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -524,7 +524,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -534,7 +534,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -544,7 +544,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -554,7 +554,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -564,7 +564,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -574,7 +574,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -584,7 +584,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -594,7 +594,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
updated my part for activity log
</commit_message>
<xml_diff>
--- a/Agora Team Activity Log.xlsx
+++ b/Agora Team Activity Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df8c00b68312d67f/University 2020 S2/INFO301/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cedricstephani/Documents/INFO301/agora_student_marketplace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{486100A1-C139-4CF8-9454-35E6B6BB17A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA57B641-6B23-3549-806E-D6431A065733}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="14280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="14280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Week 1</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Gave instructions on how to download Microsoft Visual Code, ReactJS, Node.JS and MongoDB. Create starting React project base structure and push to Git. Ensure all group members can pull the project and run the react App in their browser. Assist with scheduling and delegating of stories.</t>
+  </si>
+  <si>
+    <t>Downloaded the systems programs like Visual Code, ReactJS/NodeJS, and MongoDB. Worked on user stories and project scheduling as well as started working on a rough database model which reflects systems/user stories needs.</t>
   </si>
 </sst>
 </file>
@@ -427,14 +430,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="36.6640625" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="6" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
@@ -452,7 +455,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -472,7 +475,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -492,19 +495,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -514,7 +519,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -524,7 +529,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -534,7 +539,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -544,7 +549,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -554,7 +559,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -564,7 +569,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -574,7 +579,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -584,7 +589,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -594,7 +599,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Vainui: Updated activity log for week three.
</commit_message>
<xml_diff>
--- a/Agora Team Activity Log.xlsx
+++ b/Agora Team Activity Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\IN301\Agora Project\agora_student_marketplace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zedri\source\repos\agora_student_marketplace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF088C3-1F86-435C-9611-AB4FACDFF172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D46A49-E852-4B09-A617-00603BAA09DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Week 1</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Downloaded softwares to work in project in accordance with team plan, which are: ReactJS,NodeJS, MongoDB and Visual Studio Code. Contributed to User-Stories and Created project page on taiga.</t>
+  </si>
+  <si>
+    <t>Downloaded our chosen software for the project: ReactJS, NodeJS, MongoDB and Visual Studio Code. Have watched a few tutorials to start learning these softwares.</t>
   </si>
 </sst>
 </file>
@@ -429,18 +432,18 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="6" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="6" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
@@ -458,7 +461,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -478,7 +481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -498,7 +501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -509,12 +512,14 @@
         <v>22</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -524,7 +529,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -534,7 +539,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -544,7 +549,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -554,7 +559,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -564,7 +569,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -574,7 +579,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -584,7 +589,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -594,7 +599,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -604,7 +609,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
updated Activity log for week 3
</commit_message>
<xml_diff>
--- a/Agora Team Activity Log.xlsx
+++ b/Agora Team Activity Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zedri\source\repos\agora_student_marketplace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\IN301\Agora Project\agora_student_marketplace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D46A49-E852-4B09-A617-00603BAA09DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1111DA2C-C17C-4176-BF0B-AB133CE4E2F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,10 +91,10 @@
     <t>Downloaded the systems programs like Visual Code, ReactJS/NodeJS, and MongoDB. Worked on user stories and project scheduling as well as started working on a rough database model which reflects systems/user stories needs.</t>
   </si>
   <si>
-    <t>Downloaded softwares to work in project in accordance with team plan, which are: ReactJS,NodeJS, MongoDB and Visual Studio Code. Contributed to User-Stories and Created project page on taiga.</t>
-  </si>
-  <si>
     <t>Downloaded our chosen software for the project: ReactJS, NodeJS, MongoDB and Visual Studio Code. Have watched a few tutorials to start learning these softwares.</t>
+  </si>
+  <si>
+    <t>Downloaded softwares to work in project in accordance with team plan, which are: ReactJS,NodeJS, MongoDB and Visual Studio Code. Contributed to User-Stories and Created project page on taiga. Added Activity digram for Agora and contribute to playing planning poker with the rest of the team.</t>
   </si>
 </sst>
 </file>
@@ -433,17 +433,17 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="6" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="6" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
@@ -461,7 +461,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -481,7 +481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -501,7 +501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -513,13 +513,13 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -529,7 +529,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -539,7 +539,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -549,7 +549,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -559,7 +559,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -569,7 +569,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -579,7 +579,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -589,7 +589,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -599,7 +599,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -609,7 +609,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Working on header design.  Updated Activity Log.
</commit_message>
<xml_diff>
--- a/Agora Team Activity Log.xlsx
+++ b/Agora Team Activity Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\301\agora_student_marketplace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zedri\source\repos\agora_student_marketplace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7317AFB-3660-4E12-A7C9-DF0CDF14B08E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F3F657-85DC-421F-ABDA-7EEBA079A192}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Hugo Baird</t>
   </si>
@@ -123,13 +123,7 @@
     <t>Proposed chosen architecture pattern to team members (layered). Documented in-depth architecture section of the evidence review. Designed visual architecture model with relative components. Started focus on implementation of home screen and displaying listings. Helped other team members learning and understanding of React and set up the groundwork of the project (screen renders in App.js) to start development.</t>
   </si>
   <si>
-    <t>Set up the node js server file to pull data from the backend and serve it to the frontend. Set up a communal email and MongoDB account for the team to use. Provided instructions for team to install npm backend modules (these are in instructions.txt in the gitbucket repo). Working with Cedric to pull data from the sign up form to the backend.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created a form for the create account page which has since been put into a text file for now as we work on simplifying it until we know it works correctly. Also have set up the majority of the back end database as well as the middleware to connect these two. Just working out the final bugs with Leon before connecting it all together. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Worked on the Evidence review, watched tutorials to learn about react.js, Node js and MongoDB. Downloded dependency for as instructions to VSC and started styling front-end pages </t>
+    <t xml:space="preserve">Started front-end work regarding the main page through following tutorials suggested by the team. Helped explain the models within the feasibility study and did some proof reading/editing. Finished the heuristics document for user experience. Getting used to the new tools, so far so good. </t>
   </si>
 </sst>
 </file>
@@ -501,20 +495,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="6" width="36.7109375" customWidth="1"/>
-    <col min="7" max="1025" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="6" width="36.6640625" customWidth="1"/>
+    <col min="7" max="1025" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="24.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +526,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -552,7 +546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -572,7 +566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -592,7 +586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="104.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="103.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -612,25 +606,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="149.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="148.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -640,7 +630,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -650,7 +640,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -660,7 +650,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -670,7 +660,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -680,7 +670,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -690,7 +680,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -700,7 +690,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>